<commit_message>
Adjusted stackup to suit jlc standard stackups
</commit_message>
<xml_diff>
--- a/Output Files/Strelka_Flight_Computer_MASTER.xlsx
+++ b/Output Files/Strelka_Flight_Computer_MASTER.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thean\OneDrive\Documents\Other Projects\Strelka-Flight-Computer\Output Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thean\Documents\Other Projects\Strelka-Flight-Computer\Output Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3C88C5-2AFE-4FF1-A45D-31426C39BE32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41EF180A-C97B-4BB2-AB27-BAAB98A599A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Strelka_Flight_Computer_MASTER" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="358">
   <si>
     <t>Source:</t>
   </si>
@@ -1082,6 +1082,18 @@
   </si>
   <si>
     <t>430250208 - Molex Housing</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com.au/en/products/detail/molex/0430300001/467796?s=N4IgTCBcDaICwGYAMyloIwgLoF8g</t>
+  </si>
+  <si>
+    <t>430300001 - Crimps</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com.au/en/products/detail/stmicroelectronics/ASM330LHHXTR/16399064?s=N4IgTCBcDaIIIGUCyBmFAGAMgCWwDQBUAlEAXQF8g</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com.au/en/products/detail/te-connectivity-measurement-specialties/MS561101BA03-50/5277445</t>
   </si>
 </sst>
 </file>
@@ -1565,9 +1577,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1938,22 +1953,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L87"/>
+  <dimension ref="A1:L88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+    <sheetView tabSelected="1" topLeftCell="B69" workbookViewId="0">
+      <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="26.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.26953125" customWidth="1"/>
+    <col min="3" max="3" width="17.1796875" customWidth="1"/>
+    <col min="4" max="4" width="20.54296875" customWidth="1"/>
+    <col min="10" max="10" width="8.7265625" style="2"/>
+    <col min="11" max="11" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1961,7 +1977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1969,7 +1985,7 @@
         <v>45215.611111111109</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1977,12 +1993,12 @@
         <v>164</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2010,7 +2026,7 @@
       <c r="I7" t="s">
         <v>13</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="K7" t="s">
@@ -2020,7 +2036,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2052,7 +2068,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2</v>
       </c>
@@ -2074,7 +2090,7 @@
       <c r="G9" t="s">
         <v>25</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="2" t="s">
         <v>26</v>
       </c>
       <c r="K9" t="s">
@@ -2084,7 +2100,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>3</v>
       </c>
@@ -2116,7 +2132,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>4</v>
       </c>
@@ -2142,7 +2158,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>5</v>
       </c>
@@ -2171,7 +2187,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>6</v>
       </c>
@@ -2197,7 +2213,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>7</v>
       </c>
@@ -2223,7 +2239,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>8</v>
       </c>
@@ -2249,7 +2265,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>9</v>
       </c>
@@ -2275,7 +2291,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>10</v>
       </c>
@@ -2301,7 +2317,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>11</v>
       </c>
@@ -2333,7 +2349,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>12</v>
       </c>
@@ -2359,7 +2375,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>13</v>
       </c>
@@ -2385,7 +2401,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>14</v>
       </c>
@@ -2414,7 +2430,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>15</v>
       </c>
@@ -2440,7 +2456,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>16</v>
       </c>
@@ -2469,7 +2485,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>17</v>
       </c>
@@ -2498,7 +2514,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>18</v>
       </c>
@@ -2524,7 +2540,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>19</v>
       </c>
@@ -2553,7 +2569,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>20</v>
       </c>
@@ -2585,7 +2601,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>21</v>
       </c>
@@ -2617,7 +2633,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>22</v>
       </c>
@@ -2649,7 +2665,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>23</v>
       </c>
@@ -2681,7 +2697,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>24</v>
       </c>
@@ -2710,7 +2726,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>25</v>
       </c>
@@ -2739,7 +2755,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>26</v>
       </c>
@@ -2768,7 +2784,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>27</v>
       </c>
@@ -2797,7 +2813,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>28</v>
       </c>
@@ -2826,7 +2842,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>29</v>
       </c>
@@ -2855,7 +2871,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>30</v>
       </c>
@@ -2887,7 +2903,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>31</v>
       </c>
@@ -2916,7 +2932,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>33</v>
       </c>
@@ -2948,7 +2964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>34</v>
       </c>
@@ -2970,7 +2986,7 @@
       <c r="G40" t="s">
         <v>150</v>
       </c>
-      <c r="J40" t="s">
+      <c r="J40" s="2" t="s">
         <v>151</v>
       </c>
       <c r="K40" t="s">
@@ -2980,7 +2996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>35</v>
       </c>
@@ -3012,7 +3028,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>36</v>
       </c>
@@ -3044,7 +3060,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>37</v>
       </c>
@@ -3073,7 +3089,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>38</v>
       </c>
@@ -3102,7 +3118,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>39</v>
       </c>
@@ -3134,7 +3150,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>40</v>
       </c>
@@ -3166,7 +3182,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>41</v>
       </c>
@@ -3198,7 +3214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>42</v>
       </c>
@@ -3227,7 +3243,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>43</v>
       </c>
@@ -3259,7 +3275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>44</v>
       </c>
@@ -3291,7 +3307,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>45</v>
       </c>
@@ -3323,7 +3339,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>46</v>
       </c>
@@ -3352,7 +3368,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>47</v>
       </c>
@@ -3381,7 +3397,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>48</v>
       </c>
@@ -3410,7 +3426,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>49</v>
       </c>
@@ -3439,7 +3455,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>50</v>
       </c>
@@ -3465,7 +3481,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>51</v>
       </c>
@@ -3494,7 +3510,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>52</v>
       </c>
@@ -3523,7 +3539,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>53</v>
       </c>
@@ -3549,7 +3565,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>54</v>
       </c>
@@ -3578,7 +3594,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>55</v>
       </c>
@@ -3604,7 +3620,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>56</v>
       </c>
@@ -3633,7 +3649,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>57</v>
       </c>
@@ -3662,7 +3678,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>58</v>
       </c>
@@ -3691,7 +3707,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>59</v>
       </c>
@@ -3720,7 +3736,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>60</v>
       </c>
@@ -3752,7 +3768,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>61</v>
       </c>
@@ -3778,7 +3794,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>62</v>
       </c>
@@ -3807,7 +3823,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>63</v>
       </c>
@@ -3836,7 +3852,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>64</v>
       </c>
@@ -3865,7 +3881,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>65</v>
       </c>
@@ -3894,7 +3910,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>66</v>
       </c>
@@ -3923,7 +3939,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>67</v>
       </c>
@@ -3955,7 +3971,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>68</v>
       </c>
@@ -3987,7 +4003,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>70</v>
       </c>
@@ -4009,11 +4025,14 @@
       <c r="G75" t="s">
         <v>280</v>
       </c>
+      <c r="J75" s="2" t="s">
+        <v>356</v>
+      </c>
       <c r="K75" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>71</v>
       </c>
@@ -4045,7 +4064,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>72</v>
       </c>
@@ -4077,7 +4096,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>73</v>
       </c>
@@ -4106,7 +4125,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>74</v>
       </c>
@@ -4135,7 +4154,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>75</v>
       </c>
@@ -4164,7 +4183,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>76</v>
       </c>
@@ -4196,7 +4215,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>77</v>
       </c>
@@ -4222,10 +4241,10 @@
         <v>321</v>
       </c>
       <c r="K82" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>78</v>
       </c>
@@ -4247,11 +4266,14 @@
       <c r="G83" t="s">
         <v>326</v>
       </c>
+      <c r="J83" s="2" t="s">
+        <v>357</v>
+      </c>
       <c r="K83" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>79</v>
       </c>
@@ -4283,7 +4305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>80</v>
       </c>
@@ -4312,7 +4334,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>81</v>
       </c>
@@ -4341,7 +4363,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B87">
         <v>2</v>
       </c>
@@ -4352,8 +4374,16 @@
         <v>8</v>
       </c>
     </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="D88" t="s">
+        <v>355</v>
+      </c>
+      <c r="J88" s="2" t="s">
+        <v>354</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A8:L86 B87 D88">
+  <conditionalFormatting sqref="B87 D88 A8:L86">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Added solder paste to BOM
</commit_message>
<xml_diff>
--- a/Output Files/Strelka_Flight_Computer_MASTER.xlsx
+++ b/Output Files/Strelka_Flight_Computer_MASTER.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thean\OneDrive\Documents\Other Projects\Strelka-Flight-Computer\Output Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3C88C5-2AFE-4FF1-A45D-31426C39BE32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C04A111-B004-4159-A01C-DD9AB281BD8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Strelka_Flight_Computer_MASTER" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="355">
   <si>
     <t>Source:</t>
   </si>
@@ -1082,6 +1082,9 @@
   </si>
   <si>
     <t>430250208 - Molex Housing</t>
+  </si>
+  <si>
+    <t>Solder paste</t>
   </si>
 </sst>
 </file>
@@ -1938,10 +1941,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L87"/>
+  <dimension ref="A1:L88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="D88" sqref="D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4352,6 +4355,11 @@
         <v>8</v>
       </c>
     </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D88" t="s">
+        <v>354</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A8:L86 B87 D88">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">

</xml_diff>

<commit_message>
Adjusted bom available items
</commit_message>
<xml_diff>
--- a/Output Files/Strelka_Flight_Computer_MASTER.xlsx
+++ b/Output Files/Strelka_Flight_Computer_MASTER.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thean\OneDrive\Documents\Other Projects\Strelka-Flight-Computer\Output Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C04A111-B004-4159-A01C-DD9AB281BD8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6ED127A-E179-4B89-8DE4-C8E38C543E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1943,8 +1943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="D88" sqref="D88"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1952,6 +1952,7 @@
     <col min="2" max="2" width="26.28515625" customWidth="1"/>
     <col min="3" max="3" width="17.140625" customWidth="1"/>
     <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" customWidth="1"/>
     <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -2116,7 +2117,7 @@
         <v>346</v>
       </c>
       <c r="L10">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -3955,7 +3956,7 @@
         <v>346</v>
       </c>
       <c r="L73">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>